<commit_message>
Chrome Options Package added
</commit_message>
<xml_diff>
--- a/testdata/test2.xlsx
+++ b/testdata/test2.xlsx
@@ -970,12 +970,12 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="31.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="19.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="19.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>